<commit_message>
fix homework 3 ex 6
</commit_message>
<xml_diff>
--- a/Homework3/src/test/resources/testdata.xlsx
+++ b/Homework3/src/test/resources/testdata.xlsx
@@ -47,9 +47,6 @@
     <t>P@ssw0rd</t>
   </si>
   <si>
-    <t>Aaliyah Haq</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -59,13 +56,16 @@
     <t>testuser2</t>
   </si>
   <si>
-    <t>David Morris</t>
-  </si>
-  <si>
     <t>ESS</t>
   </si>
   <si>
     <t>Disabled</t>
+  </si>
+  <si>
+    <t>Ranga  Akunuri</t>
+  </si>
+  <si>
+    <t>Peter Mac Anderson</t>
   </si>
 </sst>
 </file>
@@ -113,12 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -404,7 +407,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,31 +436,31 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix homework 3 ex 5
</commit_message>
<xml_diff>
--- a/Homework3/src/test/resources/testdata.xlsx
+++ b/Homework3/src/test/resources/testdata.xlsx
@@ -53,7 +53,7 @@
     <t>Enabled</t>
   </si>
   <si>
-    <t>Ranga  Akunuri</t>
+    <t>Timothy Lewis Amiano</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD72"/>
+      <selection activeCell="F9" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>